<commit_message>
Added support for Claude - Untested
</commit_message>
<xml_diff>
--- a/Recursive_COT_Sandbox/Results.xlsx
+++ b/Recursive_COT_Sandbox/Results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohamsane/Documents/Coding Projects/GPT_Vision/Recursive_COT_Sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1F990F-9F35-E640-BC5C-0A99896A10F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DFA7F6-F850-2242-8E83-E21083890142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{E3495C15-F0A9-1840-9741-7182558D7961}"/>
+    <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{E3495C15-F0A9-1840-9741-7182558D7961}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="29">
   <si>
     <t>Question 1:</t>
   </si>
@@ -104,9 +104,6 @@
     <t>GPT-o1-preview</t>
   </si>
   <si>
-    <t>Claude 3.5</t>
-  </si>
-  <si>
     <t>Llama 3.1 - 405B</t>
   </si>
   <si>
@@ -114,6 +111,18 @@
   </si>
   <si>
     <t>AVERAGE EAG</t>
+  </si>
+  <si>
+    <t>GPT-o1-preview-2024-09-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Claude-3.5-Sonnet-20241022 </t>
+  </si>
+  <si>
+    <t>Llama 3.1 - 70B</t>
+  </si>
+  <si>
+    <t>Llama 3.1 - 70B - CoT Enhanced</t>
   </si>
 </sst>
 </file>
@@ -248,22 +257,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -621,6 +630,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strLit>
               <c:ptCount val="1"/>
@@ -636,7 +702,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.33999999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1152,7 +1218,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7.4999999999999997E-2</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1259,7 +1325,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.39500000000000013</c:v>
+                  <c:v>0.38500000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1294,6 +1360,63 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strLit>
               <c:ptCount val="1"/>
@@ -1309,7 +1432,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3106,8 +3229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C102F7-7C26-1043-9182-2914F0414473}">
   <dimension ref="A2:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N83" sqref="N83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3120,16 +3243,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -3174,14 +3297,14 @@
       <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="7">
         <f>AVERAGE(B4:F4)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="7">
         <f>IF(AVERAGE(B4:F4)=0, -0.25,
    IF(AVERAGE(B4:F4)&lt;=0.33, AVERAGE(B4:F4)*0.5,
-   IF(AVERAGE(B4:F4)&lt;=0.66, AVERAGE(B4:F4),
+   IF(AVERAGE(B4:F4)&lt;=0.66, AVERAGE(B4:F4)*0.75,
    AVERAGE(B4:F4)*1.5)))</f>
         <v>-0.25</v>
       </c>
@@ -3205,21 +3328,21 @@
       <c r="F5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="7">
         <f t="shared" ref="G5:G13" si="0">AVERAGE(B5:F5)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="7">
         <f t="shared" ref="H5:H13" si="1">IF(AVERAGE(B5:F5)=0, -0.25,
    IF(AVERAGE(B5:F5)&lt;=0.33, AVERAGE(B5:F5)*0.5,
-   IF(AVERAGE(B5:F5)&lt;=0.66, AVERAGE(B5:F5),
+   IF(AVERAGE(B5:F5)&lt;=0.66, AVERAGE(B5:F5)*0.75,
    AVERAGE(B5:F5)*1.5)))</f>
         <v>-0.25</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="9"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -3240,19 +3363,19 @@
       <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="7">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="7">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -3274,21 +3397,21 @@
       <c r="F7" s="2">
         <v>0</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="7">
         <f t="shared" si="1"/>
         <v>-0.25</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="7">
         <f>AVERAGE(G4:G13)</f>
         <v>0.2</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="7">
         <f>AVERAGE(H4:H13)</f>
-        <v>7.4999999999999997E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -3310,13 +3433,13 @@
       <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="7">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="7">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -3338,11 +3461,11 @@
       <c r="F9" s="2">
         <v>0</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="7">
         <f t="shared" si="1"/>
         <v>-0.25</v>
       </c>
@@ -3366,11 +3489,11 @@
       <c r="F10" s="2">
         <v>0</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="7">
         <f t="shared" si="1"/>
         <v>-0.25</v>
       </c>
@@ -3394,11 +3517,11 @@
       <c r="F11" s="2">
         <v>1</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="7">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -3422,11 +3545,11 @@
       <c r="F12" s="2">
         <v>0</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="7">
         <f t="shared" si="1"/>
         <v>-0.25</v>
       </c>
@@ -3450,26 +3573,26 @@
       <c r="F13" s="2">
         <v>0</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="7">
         <f t="shared" si="1"/>
         <v>-0.25</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
@@ -3514,14 +3637,14 @@
       <c r="F19" s="2">
         <v>1</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="7">
         <f>AVERAGE(B19:F19)</f>
         <v>0.8</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19" s="7">
         <f>IF(AVERAGE(B19:F19)=0, -0.25,
    IF(AVERAGE(B19:F19)&lt;=0.33, AVERAGE(B19:F19)*0.5,
-   IF(AVERAGE(B19:F19)&lt;=0.66, AVERAGE(B19:F19),
+   IF(AVERAGE(B19:F19)&lt;=0.66, AVERAGE(B19:F19)*0.75,
    AVERAGE(B19:F19)*1.5)))</f>
         <v>1.2000000000000002</v>
       </c>
@@ -3545,21 +3668,21 @@
       <c r="F20" s="2">
         <v>0</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="7">
         <f t="shared" ref="G20:G28" si="2">AVERAGE(B20:F20)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="7">
         <f t="shared" ref="H20:H28" si="3">IF(AVERAGE(B20:F20)=0, -0.25,
    IF(AVERAGE(B20:F20)&lt;=0.33, AVERAGE(B20:F20)*0.5,
-   IF(AVERAGE(B20:F20)&lt;=0.66, AVERAGE(B20:F20),
+   IF(AVERAGE(B20:F20)&lt;=0.66, AVERAGE(B20:F20)*0.75,
    AVERAGE(B20:F20)*1.5)))</f>
         <v>-0.25</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="J20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K20" s="9"/>
+      <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
@@ -3580,11 +3703,11 @@
       <c r="F21" s="2">
         <v>1</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="7">
         <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="7">
         <f t="shared" si="3"/>
         <v>1.2000000000000002</v>
       </c>
@@ -3592,7 +3715,7 @@
         <v>19</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -3614,21 +3737,21 @@
       <c r="F22" s="2">
         <v>0</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="7">
         <f t="shared" si="3"/>
         <v>-0.25</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="7">
         <f>AVERAGE(G19:G28)</f>
         <v>0.36</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="7">
         <f>AVERAGE(H19:H28)</f>
-        <v>0.39500000000000013</v>
+        <v>0.38500000000000006</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -3650,11 +3773,11 @@
       <c r="F23" s="2">
         <v>0</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="7">
         <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
-      <c r="H23" s="10">
+      <c r="H23" s="7">
         <f t="shared" si="3"/>
         <v>1.2000000000000002</v>
       </c>
@@ -3678,11 +3801,11 @@
       <c r="F24" s="2">
         <v>0</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="7">
         <f t="shared" si="3"/>
         <v>-0.25</v>
       </c>
@@ -3706,11 +3829,11 @@
       <c r="F25" s="2">
         <v>0</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="7">
         <f t="shared" si="3"/>
         <v>-0.25</v>
       </c>
@@ -3734,11 +3857,11 @@
       <c r="F26" s="2">
         <v>1</v>
       </c>
-      <c r="G26" s="10">
+      <c r="G26" s="7">
         <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="7">
         <f t="shared" si="3"/>
         <v>1.2000000000000002</v>
       </c>
@@ -3762,13 +3885,13 @@
       <c r="F27" s="2">
         <v>1</v>
       </c>
-      <c r="G27" s="10">
+      <c r="G27" s="7">
         <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-      <c r="H27" s="10">
+      <c r="H27" s="7">
         <f t="shared" si="3"/>
-        <v>0.4</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -3790,11 +3913,11 @@
       <c r="F28" s="2">
         <v>0</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28" s="7">
         <f t="shared" si="3"/>
         <v>-0.25</v>
       </c>
@@ -3803,16 +3926,16 @@
       <c r="A31" s="4"/>
     </row>
     <row r="32" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="A32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
@@ -3842,217 +3965,317 @@
       <c r="A34" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="10" t="e">
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="7">
         <f>AVERAGE(B34:F34)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H34" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H34" s="7">
         <f>IF(AVERAGE(B34:F34)=0, -0.25,
    IF(AVERAGE(B34:F34)&lt;=0.33, AVERAGE(B34:F34)*0.5,
-   IF(AVERAGE(B34:F34)&lt;=0.66, AVERAGE(B34:F34),
+   IF(AVERAGE(B34:F34)&lt;=0.66, AVERAGE(B34:F34)*0.75,
    AVERAGE(B34:F34)*1.5)))</f>
-        <v>#DIV/0!</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="10" t="e">
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="7">
         <f t="shared" ref="G35:G43" si="4">AVERAGE(B35:F35)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H35" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H35" s="7">
         <f t="shared" ref="H35:H43" si="5">IF(AVERAGE(B35:F35)=0, -0.25,
    IF(AVERAGE(B35:F35)&lt;=0.33, AVERAGE(B35:F35)*0.5,
-   IF(AVERAGE(B35:F35)&lt;=0.66, AVERAGE(B35:F35),
+   IF(AVERAGE(B35:F35)&lt;=0.66, AVERAGE(B35:F35)*0.75,
    AVERAGE(B35:F35)*1.5)))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J35" s="9" t="s">
+        <v>-0.25</v>
+      </c>
+      <c r="J35" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K35" s="9"/>
+      <c r="K35" s="8"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="10" t="e">
+      <c r="B36" s="2">
+        <v>0</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0</v>
+      </c>
+      <c r="G36" s="7">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H36" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H36" s="7">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-0.25</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="10" t="e">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="7">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H37" s="10" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="H37" s="7">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J37" s="10" t="e">
+        <v>0.1</v>
+      </c>
+      <c r="J37" s="7">
         <f>AVERAGE(G34:G43)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K37" s="10" t="e">
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="K37" s="7">
         <f>AVERAGE(H34:H43)</f>
-        <v>#DIV/0!</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="10" t="e">
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1</v>
+      </c>
+      <c r="G38" s="7">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H38" s="10" t="e">
+        <v>1</v>
+      </c>
+      <c r="H38" s="7">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="10" t="e">
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
+      <c r="G39" s="7">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H39" s="10" t="e">
+        <v>0.6</v>
+      </c>
+      <c r="H39" s="7">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="10" t="e">
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0</v>
+      </c>
+      <c r="G40" s="7">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H40" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H40" s="7">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="10" t="e">
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1</v>
+      </c>
+      <c r="G41" s="7">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H41" s="10" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="H41" s="7">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1.2000000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="10" t="e">
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1</v>
+      </c>
+      <c r="G42" s="7">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H42" s="10" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="H42" s="7">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>1.2000000000000002</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="10" t="e">
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0</v>
+      </c>
+      <c r="G43" s="7">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H43" s="10" t="e">
+        <v>0</v>
+      </c>
+      <c r="H43" s="7">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
+      <c r="A47" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
@@ -4087,12 +4310,15 @@
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="10" t="e">
+      <c r="G49" s="7" t="e">
         <f>AVERAGE(B49:F49)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H49" s="10" t="e">
-        <f>IF(AVERAGE(B49:F49)&lt;=0.33, AVERAGE(B49:F49)*0.5, IF(AVERAGE(B49:F49)&lt;=0.66, AVERAGE(B49:F49), AVERAGE(B49:F49)*1.5))</f>
+      <c r="H49" s="7" t="e">
+        <f>IF(AVERAGE(B49:F49)=0, -0.25,
+   IF(AVERAGE(B49:F49)&lt;=0.33, AVERAGE(B49:F49)*0.5,
+   IF(AVERAGE(B49:F49)&lt;=0.66, AVERAGE(B49:F49)*0.75,
+   AVERAGE(B49:F49)*1.5)))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4105,18 +4331,21 @@
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="10" t="e">
+      <c r="G50" s="7" t="e">
         <f t="shared" ref="G50:G58" si="6">AVERAGE(B50:F50)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H50" s="10" t="e">
-        <f t="shared" ref="H50:H58" si="7">IF(AVERAGE(B50:F50)&lt;=0.33, AVERAGE(B50:F50)*0.5, IF(AVERAGE(B50:F50)&lt;=0.66, AVERAGE(B50:F50), AVERAGE(B50:F50)*1.5))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J50" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K50" s="9"/>
+      <c r="H50" s="7" t="e">
+        <f t="shared" ref="H50:H58" si="7">IF(AVERAGE(B50:F50)=0, -0.25,
+   IF(AVERAGE(B50:F50)&lt;=0.33, AVERAGE(B50:F50)*0.5,
+   IF(AVERAGE(B50:F50)&lt;=0.66, AVERAGE(B50:F50)*0.75,
+   AVERAGE(B50:F50)*1.5)))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J50" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K50" s="8"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
@@ -4127,11 +4356,11 @@
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="10" t="e">
+      <c r="G51" s="7" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H51" s="10" t="e">
+      <c r="H51" s="7" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
@@ -4151,20 +4380,20 @@
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="10" t="e">
+      <c r="G52" s="7" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H52" s="10" t="e">
+      <c r="H52" s="7" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J52" s="10" t="e">
+      <c r="J52" s="7" t="e">
         <f>AVERAGE(G49:G58)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K52" s="10" t="e">
-        <f>IF(AVERAGE(H49:H58)&lt;=0.33, AVERAGE(H49:H58)*0.5, IF(AVERAGE(H49:H58)&lt;=0.66, AVERAGE(H49:H58), AVERAGE(H49:H58)*1.5))</f>
+      <c r="K52" s="7" t="e">
+        <f>AVERAGE(H49:H58)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4177,11 +4406,11 @@
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="10" t="e">
+      <c r="G53" s="7" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H53" s="10" t="e">
+      <c r="H53" s="7" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
@@ -4195,11 +4424,11 @@
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
-      <c r="G54" s="10" t="e">
+      <c r="G54" s="7" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H54" s="10" t="e">
+      <c r="H54" s="7" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
@@ -4213,11 +4442,11 @@
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-      <c r="G55" s="10" t="e">
+      <c r="G55" s="7" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H55" s="10" t="e">
+      <c r="H55" s="7" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
@@ -4231,11 +4460,11 @@
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="10" t="e">
+      <c r="G56" s="7" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H56" s="10" t="e">
+      <c r="H56" s="7" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
@@ -4249,11 +4478,11 @@
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
-      <c r="G57" s="10" t="e">
+      <c r="G57" s="7" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H57" s="10" t="e">
+      <c r="H57" s="7" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
@@ -4267,26 +4496,26 @@
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="10" t="e">
+      <c r="G58" s="7" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H58" s="10" t="e">
+      <c r="H58" s="7" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A62" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
+      <c r="A62" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
@@ -4321,12 +4550,15 @@
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-      <c r="G64" s="10" t="e">
+      <c r="G64" s="7" t="e">
         <f>AVERAGE(B64:F64)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H64" s="10" t="e">
-        <f>IF(AVERAGE(B64:F64)&lt;=0.33, AVERAGE(B64:F64)*0.5, IF(AVERAGE(B64:F64)&lt;=0.66, AVERAGE(B64:F64), AVERAGE(B64:F64)*1.5))</f>
+      <c r="H64" s="7" t="e">
+        <f>IF(AVERAGE(B64:F64)=0, -0.25,
+   IF(AVERAGE(B64:F64)&lt;=0.33, AVERAGE(B64:F64)*0.5,
+   IF(AVERAGE(B64:F64)&lt;=0.66, AVERAGE(B64:F64)*0.75,
+   AVERAGE(B64:F64)*1.5)))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4339,18 +4571,21 @@
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="10" t="e">
+      <c r="G65" s="7" t="e">
         <f t="shared" ref="G65:G73" si="8">AVERAGE(B65:F65)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H65" s="10" t="e">
-        <f t="shared" ref="H65:H73" si="9">IF(AVERAGE(B65:F65)&lt;=0.33, AVERAGE(B65:F65)*0.5, IF(AVERAGE(B65:F65)&lt;=0.66, AVERAGE(B65:F65), AVERAGE(B65:F65)*1.5))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J65" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K65" s="9"/>
+      <c r="H65" s="7" t="e">
+        <f t="shared" ref="H65:H73" si="9">IF(AVERAGE(B65:F65)=0, -0.25,
+   IF(AVERAGE(B65:F65)&lt;=0.33, AVERAGE(B65:F65)*0.5,
+   IF(AVERAGE(B65:F65)&lt;=0.66, AVERAGE(B65:F65)*0.75,
+   AVERAGE(B65:F65)*1.5)))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J65" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K65" s="8"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
@@ -4361,11 +4596,11 @@
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
-      <c r="G66" s="10" t="e">
+      <c r="G66" s="7" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H66" s="10" t="e">
+      <c r="H66" s="7" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -4385,20 +4620,20 @@
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
-      <c r="G67" s="10" t="e">
+      <c r="G67" s="7" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H67" s="10" t="e">
+      <c r="H67" s="7" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J67" s="10" t="e">
+      <c r="J67" s="7" t="e">
         <f>AVERAGE(G64:G73)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K67" s="10" t="e">
-        <f>IF(AVERAGE(H64:H73)&lt;=0.33, AVERAGE(H64:H73)*0.5, IF(AVERAGE(H64:H73)&lt;=0.66, AVERAGE(H64:H73), AVERAGE(H64:H73)*1.5))</f>
+      <c r="K67" s="7" t="e">
+        <f>AVERAGE(H64:H73)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4411,11 +4646,11 @@
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
-      <c r="G68" s="10" t="e">
+      <c r="G68" s="7" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H68" s="10" t="e">
+      <c r="H68" s="7" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -4429,11 +4664,11 @@
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
-      <c r="G69" s="10" t="e">
+      <c r="G69" s="7" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H69" s="10" t="e">
+      <c r="H69" s="7" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -4447,11 +4682,11 @@
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
-      <c r="G70" s="10" t="e">
+      <c r="G70" s="7" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H70" s="10" t="e">
+      <c r="H70" s="7" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -4465,11 +4700,11 @@
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
-      <c r="G71" s="10" t="e">
+      <c r="G71" s="7" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H71" s="10" t="e">
+      <c r="H71" s="7" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -4483,11 +4718,11 @@
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
-      <c r="G72" s="10" t="e">
+      <c r="G72" s="7" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H72" s="10" t="e">
+      <c r="H72" s="7" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
@@ -4501,26 +4736,26 @@
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
-      <c r="G73" s="10" t="e">
+      <c r="G73" s="7" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H73" s="10" t="e">
+      <c r="H73" s="7" t="e">
         <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A77" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
-      <c r="F77" s="8"/>
-      <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
+      <c r="A77" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
@@ -4555,12 +4790,15 @@
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
-      <c r="G79" s="10" t="e">
+      <c r="G79" s="7" t="e">
         <f>AVERAGE(B79:F79)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H79" s="10" t="e">
-        <f>IF(AVERAGE(B79:F79)&lt;=0.33, AVERAGE(B79:F79)*0.5, IF(AVERAGE(B79:F79)&lt;=0.66, AVERAGE(B79:F79), AVERAGE(B79:F79)*1.5))</f>
+      <c r="H79" s="7" t="e">
+        <f>IF(AVERAGE(B79:F79)=0, -0.25,
+   IF(AVERAGE(B79:F79)&lt;=0.33, AVERAGE(B79:F79)*0.5,
+   IF(AVERAGE(B79:F79)&lt;=0.66, AVERAGE(B79:F79)*0.75,
+   AVERAGE(B79:F79)*1.5)))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4573,18 +4811,21 @@
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
-      <c r="G80" s="10" t="e">
+      <c r="G80" s="7" t="e">
         <f t="shared" ref="G80:G88" si="10">AVERAGE(B80:F80)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H80" s="10" t="e">
-        <f t="shared" ref="H80:H88" si="11">IF(AVERAGE(B80:F80)&lt;=0.33, AVERAGE(B80:F80)*0.5, IF(AVERAGE(B80:F80)&lt;=0.66, AVERAGE(B80:F80), AVERAGE(B80:F80)*1.5))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J80" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K80" s="9"/>
+      <c r="H80" s="7" t="e">
+        <f t="shared" ref="H80:H88" si="11">IF(AVERAGE(B80:F80)=0, -0.25,
+   IF(AVERAGE(B80:F80)&lt;=0.33, AVERAGE(B80:F80)*0.5,
+   IF(AVERAGE(B80:F80)&lt;=0.66, AVERAGE(B80:F80)*0.75,
+   AVERAGE(B80:F80)*1.5)))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J80" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K80" s="8"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
@@ -4595,11 +4836,11 @@
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
-      <c r="G81" s="10" t="e">
+      <c r="G81" s="7" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H81" s="10" t="e">
+      <c r="H81" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
@@ -4619,20 +4860,20 @@
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
-      <c r="G82" s="10" t="e">
+      <c r="G82" s="7" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H82" s="10" t="e">
+      <c r="H82" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J82" s="10" t="e">
+      <c r="J82" s="7" t="e">
         <f>AVERAGE(G79:G88)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K82" s="10" t="e">
-        <f>IF(AVERAGE(H79:H88)&lt;=0.33, AVERAGE(H79:H88)*0.5, IF(AVERAGE(H79:H88)&lt;=0.66, AVERAGE(H79:H88), AVERAGE(H79:H88)*1.5))</f>
+      <c r="K82" s="7" t="e">
+        <f>AVERAGE(H79:H88)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -4645,11 +4886,11 @@
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
-      <c r="G83" s="10" t="e">
+      <c r="G83" s="7" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H83" s="10" t="e">
+      <c r="H83" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
@@ -4663,11 +4904,11 @@
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
-      <c r="G84" s="10" t="e">
+      <c r="G84" s="7" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H84" s="10" t="e">
+      <c r="H84" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
@@ -4681,11 +4922,11 @@
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
-      <c r="G85" s="10" t="e">
+      <c r="G85" s="7" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H85" s="10" t="e">
+      <c r="H85" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
@@ -4699,11 +4940,11 @@
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
-      <c r="G86" s="10" t="e">
+      <c r="G86" s="7" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H86" s="10" t="e">
+      <c r="H86" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
@@ -4717,11 +4958,11 @@
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
-      <c r="G87" s="10" t="e">
+      <c r="G87" s="7" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H87" s="10" t="e">
+      <c r="H87" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
@@ -4735,17 +4976,22 @@
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
-      <c r="G88" s="10" t="e">
+      <c r="G88" s="7" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H88" s="10" t="e">
+      <c r="H88" s="7" t="e">
         <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="J80:K80"/>
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="A47:H47"/>
@@ -4753,11 +4999,6 @@
     <mergeCell ref="A62:H62"/>
     <mergeCell ref="J65:K65"/>
     <mergeCell ref="A77:H77"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added functionality for Claude API + Documents Update
</commit_message>
<xml_diff>
--- a/Recursive_COT_Sandbox/Results.xlsx
+++ b/Recursive_COT_Sandbox/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohamsane/Documents/Coding Projects/GPT_Vision/Recursive_COT_Sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DFA7F6-F850-2242-8E83-E21083890142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD41586-8731-9C48-8969-BAA4B953CEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{E3495C15-F0A9-1840-9741-7182558D7961}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E3495C15-F0A9-1840-9741-7182558D7961}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="28">
   <si>
     <t>Question 1:</t>
   </si>
@@ -104,12 +104,6 @@
     <t>GPT-o1-preview</t>
   </si>
   <si>
-    <t>Llama 3.1 - 405B</t>
-  </si>
-  <si>
-    <t>Llama 3.1 - 405B - CoT Enhanced</t>
-  </si>
-  <si>
     <t>AVERAGE EAG</t>
   </si>
   <si>
@@ -119,10 +113,13 @@
     <t xml:space="preserve">Claude-3.5-Sonnet-20241022 </t>
   </si>
   <si>
-    <t>Llama 3.1 - 70B</t>
+    <t xml:space="preserve">Claude-3.5-Sonnet-2024-10-22 </t>
   </si>
   <si>
-    <t>Llama 3.1 - 70B - CoT Enhanced</t>
+    <t>Claude-3-Opus-2024-02-29</t>
+  </si>
+  <si>
+    <t>Claude-3-Opus-2024-02-29- CoT Enhanced</t>
   </si>
 </sst>
 </file>
@@ -314,7 +311,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -327,14 +324,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1"/>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
               <a:t>Total AVG@5</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" b="1" baseline="0"/>
               <a:t> Results</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" b="1"/>
+            <a:endParaRPr lang="en-US" sz="1800" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -359,7 +356,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -431,7 +428,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -538,7 +535,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -645,7 +642,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -710,6 +707,105 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-BD21-6E45-A13E-83CFAE75250A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Claude-3.5-Sonnet-20241022 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$52</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D0B-4AE8-9FD6-4B8969EA9879}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -782,7 +878,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -847,7 +943,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -860,7 +956,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
                   <a:t>Total AVG@5</a:t>
                 </a:r>
               </a:p>
@@ -879,7 +975,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -911,7 +1007,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -955,7 +1051,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1036,7 +1132,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1049,22 +1145,22 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1"/>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
               <a:t>AVERAGE</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" b="1" baseline="0"/>
               <a:t> EAG</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" b="1"/>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
               <a:t>@5</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:rPr lang="en-US" sz="1800" b="1" baseline="0"/>
               <a:t> Results</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" b="1"/>
+            <a:endParaRPr lang="en-US" sz="1800" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1089,7 +1185,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1161,7 +1257,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1268,7 +1364,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1375,7 +1471,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1440,6 +1536,105 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-212A-CA46-9587-DA0D67A66BD3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Claude-3.5-Sonnet-20241022 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$52</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.66500000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6529-418F-B941-B7BCEFA56221}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1512,7 +1707,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1577,7 +1772,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1590,7 +1785,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:rPr lang="en-US" sz="1400" b="1"/>
                   <a:t>AVERAGE EAG@5</a:t>
                 </a:r>
               </a:p>
@@ -1609,7 +1804,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1641,7 +1836,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1685,7 +1880,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2836,15 +3031,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>544195</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>206829</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>86995</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2872,15 +3067,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>617038</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>34562</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>241390</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>52433</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3229,11 +3424,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C102F7-7C26-1043-9182-2914F0414473}">
   <dimension ref="A2:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N83" sqref="N83"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="112" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N75" sqref="N75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" style="1" customWidth="1"/>
     <col min="2" max="8" width="10.83203125" style="1"/>
@@ -3375,7 +3570,7 @@
         <v>19</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -3715,7 +3910,7 @@
         <v>19</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -3927,7 +4122,7 @@
     </row>
     <row r="32" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -4058,7 +4253,7 @@
         <v>19</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -4267,7 +4462,7 @@
     </row>
     <row r="47" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -4305,45 +4500,65 @@
       <c r="A49" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="7" t="e">
+      <c r="B49" s="2">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1</v>
+      </c>
+      <c r="F49" s="2">
+        <v>1</v>
+      </c>
+      <c r="G49" s="7">
         <f>AVERAGE(B49:F49)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H49" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="H49" s="7">
         <f>IF(AVERAGE(B49:F49)=0, -0.25,
    IF(AVERAGE(B49:F49)&lt;=0.33, AVERAGE(B49:F49)*0.5,
    IF(AVERAGE(B49:F49)&lt;=0.66, AVERAGE(B49:F49)*0.75,
    AVERAGE(B49:F49)*1.5)))</f>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="7" t="e">
+      <c r="B50" s="2">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1</v>
+      </c>
+      <c r="F50" s="2">
+        <v>1</v>
+      </c>
+      <c r="G50" s="7">
         <f t="shared" ref="G50:G58" si="6">AVERAGE(B50:F50)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H50" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="H50" s="7">
         <f t="shared" ref="H50:H58" si="7">IF(AVERAGE(B50:F50)=0, -0.25,
    IF(AVERAGE(B50:F50)&lt;=0.33, AVERAGE(B50:F50)*0.5,
    IF(AVERAGE(B50:F50)&lt;=0.66, AVERAGE(B50:F50)*0.75,
    AVERAGE(B50:F50)*1.5)))</f>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K50" s="8"/>
     </row>
@@ -4351,18 +4566,28 @@
       <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="7" t="e">
+      <c r="B51" s="2">
+        <v>0</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0</v>
+      </c>
+      <c r="G51" s="7">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H51" s="7" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="H51" s="7">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>0.1</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>19</v>
@@ -4375,139 +4600,209 @@
       <c r="A52" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="7" t="e">
+      <c r="B52" s="2">
+        <v>0</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0</v>
+      </c>
+      <c r="G52" s="7">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H52" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="H52" s="7">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J52" s="7" t="e">
+        <v>-0.25</v>
+      </c>
+      <c r="J52" s="7">
         <f>AVERAGE(G49:G58)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K52" s="7" t="e">
+        <v>0.52</v>
+      </c>
+      <c r="K52" s="7">
         <f>AVERAGE(H49:H58)</f>
-        <v>#DIV/0!</v>
+        <v>0.66500000000000004</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="7" t="e">
+      <c r="B53" s="2">
+        <v>0</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1</v>
+      </c>
+      <c r="F53" s="2">
+        <v>1</v>
+      </c>
+      <c r="G53" s="7">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H53" s="7" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="H53" s="7">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>1.2000000000000002</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="7" t="e">
+      <c r="B54" s="2">
+        <v>0</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0</v>
+      </c>
+      <c r="G54" s="7">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H54" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="H54" s="7">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="7" t="e">
+      <c r="B55" s="2">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
+      <c r="G55" s="7">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H55" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="H55" s="7">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="7" t="e">
+      <c r="B56" s="2">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2">
+        <v>1</v>
+      </c>
+      <c r="G56" s="7">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H56" s="7" t="e">
+        <v>1</v>
+      </c>
+      <c r="H56" s="7">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="7" t="e">
+      <c r="B57" s="2">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0</v>
+      </c>
+      <c r="G57" s="7">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H57" s="7" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="H57" s="7">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="7" t="e">
+      <c r="B58" s="2">
+        <v>0</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0</v>
+      </c>
+      <c r="G58" s="7">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H58" s="7" t="e">
+        <v>0</v>
+      </c>
+      <c r="H58" s="7">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
@@ -4583,7 +4878,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J65" s="8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K65" s="8"/>
     </row>
@@ -4747,7 +5042,7 @@
     </row>
     <row r="77" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
@@ -4823,7 +5118,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="J80" s="8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="K80" s="8"/>
     </row>
@@ -5004,4 +5299,10 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{4447dd6a-a4a1-440b-a6a3-9124ef1ee017}" enabled="1" method="Privileged" siteId="{7a18110d-ef9b-4274-acef-e62ab0fe28ed}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Document Updates & New Graphing Updates
</commit_message>
<xml_diff>
--- a/Recursive_COT_Sandbox/Results.xlsx
+++ b/Recursive_COT_Sandbox/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohamsane/Documents/Coding Projects/GPT_Vision/Recursive_COT_Sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1E5061-C595-3A48-BABE-D839082E785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AD7678-ADBD-D040-85F7-7D54DE9F1550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{E3495C15-F0A9-1840-9741-7182558D7961}"/>
   </bookViews>
@@ -501,7 +501,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$20</c:f>
+              <c:f>Sheet1!$J$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -587,7 +587,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$22</c:f>
+              <c:f>Sheet1!$J$10</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -608,7 +608,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$35</c:f>
+              <c:f>Sheet1!$J$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -694,7 +694,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$37</c:f>
+              <c:f>Sheet1!$J$13</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -715,7 +715,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$50</c:f>
+              <c:f>Sheet1!$J$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -793,7 +793,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$52</c:f>
+              <c:f>Sheet1!$J$16</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -814,7 +814,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$80</c:f>
+              <c:f>Sheet1!$J$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -892,7 +892,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$82</c:f>
+              <c:f>Sheet1!$J$22</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -913,7 +913,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$65</c:f>
+              <c:f>Sheet1!$J$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -991,7 +991,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$67</c:f>
+              <c:f>Sheet1!$J$19</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1538,7 +1538,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$20</c:f>
+              <c:f>Sheet1!$J$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1624,7 +1624,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$22</c:f>
+              <c:f>Sheet1!$K$10</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1645,7 +1645,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$35</c:f>
+              <c:f>Sheet1!$J$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1731,7 +1731,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$37</c:f>
+              <c:f>Sheet1!$K$13</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1752,7 +1752,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$50</c:f>
+              <c:f>Sheet1!$J$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1830,7 +1830,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$52</c:f>
+              <c:f>Sheet1!$K$16</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1851,7 +1851,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$80</c:f>
+              <c:f>Sheet1!$J$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1929,7 +1929,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$82</c:f>
+              <c:f>Sheet1!$K$22</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1950,7 +1950,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$65</c:f>
+              <c:f>Sheet1!$J$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2028,7 +2028,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$67</c:f>
+              <c:f>Sheet1!$K$19</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -3841,7 +3841,7 @@
   <dimension ref="A2:K88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4052,6 +4052,10 @@
         <f t="shared" si="1"/>
         <v>0.44999999999999996</v>
       </c>
+      <c r="J8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -4083,6 +4087,12 @@
    AVERAGE(B9:F9)*1.5)))</f>
         <v>-0.25</v>
       </c>
+      <c r="J9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -4111,6 +4121,14 @@
         <f t="shared" si="1"/>
         <v>-0.25</v>
       </c>
+      <c r="J10" s="7">
+        <f>AVERAGE(G19:G28)</f>
+        <v>0.36</v>
+      </c>
+      <c r="K10" s="7">
+        <f>AVERAGE(H19:H28)</f>
+        <v>0.38500000000000006</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -4139,6 +4157,10 @@
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
+      <c r="J11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -4167,6 +4189,12 @@
         <f t="shared" si="1"/>
         <v>-0.25</v>
       </c>
+      <c r="J12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -4194,6 +4222,38 @@
       <c r="H13" s="7">
         <f t="shared" si="1"/>
         <v>-0.25</v>
+      </c>
+      <c r="J13" s="7">
+        <f>AVERAGE(G34:G43)</f>
+        <v>0.33999999999999997</v>
+      </c>
+      <c r="K13" s="7">
+        <f>AVERAGE(H34:H43)</f>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J16" s="7">
+        <f>AVERAGE(G49:G58)</f>
+        <v>0.52</v>
+      </c>
+      <c r="K16" s="7">
+        <f>AVERAGE(H49:H58)</f>
+        <v>0.66500000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="18" x14ac:dyDescent="0.2">
@@ -4207,6 +4267,10 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
+      <c r="J17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
@@ -4230,6 +4294,12 @@
       </c>
       <c r="H18" s="6" t="s">
         <v>15</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -4262,6 +4332,14 @@
    AVERAGE(B19:F19)*1.5)))</f>
         <v>1.2000000000000002</v>
       </c>
+      <c r="J19" s="7">
+        <f>AVERAGE(G64:G73)</f>
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="K19" s="7">
+        <f>AVERAGE(H64:H73)</f>
+        <v>0.13500000000000001</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
@@ -4294,7 +4372,7 @@
         <v>-0.25</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K20" s="8"/>
     </row>
@@ -4329,7 +4407,7 @@
         <v>19</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -4360,12 +4438,12 @@
         <v>-0.25</v>
       </c>
       <c r="J22" s="7">
-        <f>AVERAGE(G19:G28)</f>
-        <v>0.36</v>
+        <f>AVERAGE(G79:G88)</f>
+        <v>0.42000000000000004</v>
       </c>
       <c r="K22" s="7">
-        <f>AVERAGE(H19:H28)</f>
-        <v>0.38500000000000006</v>
+        <f>AVERAGE(H79:H88)</f>
+        <v>0.47499999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -4551,7 +4629,7 @@
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="3" t="s">
         <v>10</v>
@@ -4575,7 +4653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>0</v>
       </c>
@@ -4606,7 +4684,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>1</v>
       </c>
@@ -4636,12 +4714,8 @@
    AVERAGE(B35:F35)*1.5)))</f>
         <v>-0.25</v>
       </c>
-      <c r="J35" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K35" s="8"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
@@ -4668,14 +4742,8 @@
         <f t="shared" si="5"/>
         <v>-0.25</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>3</v>
       </c>
@@ -4702,16 +4770,8 @@
         <f t="shared" si="5"/>
         <v>0.1</v>
       </c>
-      <c r="J37" s="7">
-        <f>AVERAGE(G34:G43)</f>
-        <v>0.33999999999999997</v>
-      </c>
-      <c r="K37" s="7">
-        <f>AVERAGE(H34:H43)</f>
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>4</v>
       </c>
@@ -4739,7 +4799,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>5</v>
       </c>
@@ -4767,7 +4827,7 @@
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>6</v>
       </c>
@@ -4795,7 +4855,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -4823,7 +4883,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>8</v>
       </c>
@@ -4851,7 +4911,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>9</v>
       </c>
@@ -4879,7 +4939,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>25</v>
       </c>
@@ -4891,7 +4951,7 @@
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="3" t="s">
         <v>10</v>
@@ -4915,7 +4975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>0</v>
       </c>
@@ -4946,7 +5006,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>1</v>
       </c>
@@ -4976,12 +5036,8 @@
    AVERAGE(B50:F50)*1.5)))</f>
         <v>1.5</v>
       </c>
-      <c r="J50" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K50" s="8"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
@@ -5008,14 +5064,8 @@
         <f t="shared" si="7"/>
         <v>0.1</v>
       </c>
-      <c r="J51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>3</v>
       </c>
@@ -5042,16 +5092,8 @@
         <f t="shared" si="7"/>
         <v>-0.25</v>
       </c>
-      <c r="J52" s="7">
-        <f>AVERAGE(G49:G58)</f>
-        <v>0.52</v>
-      </c>
-      <c r="K52" s="7">
-        <f>AVERAGE(H49:H58)</f>
-        <v>0.66500000000000004</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>4</v>
       </c>
@@ -5079,7 +5121,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>5</v>
       </c>
@@ -5107,7 +5149,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>6</v>
       </c>
@@ -5135,7 +5177,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>7</v>
       </c>
@@ -5163,7 +5205,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>8</v>
       </c>
@@ -5191,7 +5233,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>9</v>
       </c>
@@ -5219,7 +5261,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
         <v>26</v>
       </c>
@@ -5231,7 +5273,7 @@
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="3" t="s">
         <v>10</v>
@@ -5255,7 +5297,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>0</v>
       </c>
@@ -5286,7 +5328,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>1</v>
       </c>
@@ -5316,12 +5358,8 @@
    AVERAGE(B65:F65)*1.5)))</f>
         <v>-0.25</v>
       </c>
-      <c r="J65" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K65" s="8"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>2</v>
       </c>
@@ -5348,14 +5386,8 @@
         <f t="shared" si="9"/>
         <v>-0.25</v>
       </c>
-      <c r="J66" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K66" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>3</v>
       </c>
@@ -5382,16 +5414,8 @@
         <f t="shared" si="9"/>
         <v>-0.25</v>
       </c>
-      <c r="J67" s="7">
-        <f>AVERAGE(G64:G73)</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="K67" s="7">
-        <f>AVERAGE(H64:H73)</f>
-        <v>0.13500000000000001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>4</v>
       </c>
@@ -5419,7 +5443,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>5</v>
       </c>
@@ -5447,7 +5471,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>6</v>
       </c>
@@ -5475,7 +5499,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>7</v>
       </c>
@@ -5503,7 +5527,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>8</v>
       </c>
@@ -5531,7 +5555,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>9</v>
       </c>
@@ -5559,7 +5583,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>27</v>
       </c>
@@ -5571,7 +5595,7 @@
       <c r="G77" s="10"/>
       <c r="H77" s="10"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="3" t="s">
         <v>10</v>
@@ -5595,7 +5619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>0</v>
       </c>
@@ -5626,7 +5650,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>1</v>
       </c>
@@ -5656,12 +5680,8 @@
    AVERAGE(B80:F80)*1.5)))</f>
         <v>-0.25</v>
       </c>
-      <c r="J80" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K80" s="8"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>2</v>
       </c>
@@ -5688,14 +5708,8 @@
         <f t="shared" si="11"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="J81" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K81" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
@@ -5722,16 +5736,8 @@
         <f t="shared" si="11"/>
         <v>-0.25</v>
       </c>
-      <c r="J82" s="7">
-        <f>AVERAGE(G79:G88)</f>
-        <v>0.42000000000000004</v>
-      </c>
-      <c r="K82" s="7">
-        <f>AVERAGE(H79:H88)</f>
-        <v>0.47499999999999998</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>4</v>
       </c>
@@ -5759,7 +5765,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>5</v>
       </c>
@@ -5787,7 +5793,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>6</v>
       </c>
@@ -5815,7 +5821,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>7</v>
       </c>
@@ -5843,7 +5849,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>8</v>
       </c>
@@ -5871,7 +5877,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>9</v>
       </c>
@@ -5902,16 +5908,16 @@
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A17:H17"/>
-    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J8:K8"/>
     <mergeCell ref="A32:H32"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J80:K80"/>
-    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J11:K11"/>
     <mergeCell ref="A47:H47"/>
-    <mergeCell ref="J50:K50"/>
+    <mergeCell ref="J14:K14"/>
     <mergeCell ref="A62:H62"/>
-    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="J17:K17"/>
     <mergeCell ref="A77:H77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>